<commit_message>
Updated due to the addition of the aperture
</commit_message>
<xml_diff>
--- a/aplicação/tabela_exemplo.xlsx
+++ b/aplicação/tabela_exemplo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diogo\Desktop\new_tese_after_git\eletronica\SMU\my_stuff\final_GUI\GUI-and-data-analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diogo\Desktop\dissertacao\aplicação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F8B2AE-F298-474E-B683-2C7ECD9064ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC5387D-FF09-4E40-BB4B-9D14939E23F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="31">
   <si>
     <t>name</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>20</t>
+  </si>
+  <si>
+    <t>Aperture</t>
   </si>
 </sst>
 </file>
@@ -440,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="F2" sqref="F2:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -451,7 +454,7 @@
     <col min="2" max="3" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -468,31 +471,34 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -508,32 +514,35 @@
       <c r="E2" s="1">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="F2">
-        <v>-0.5</v>
+      <c r="F2" s="1">
+        <v>1</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="H2">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="I2">
-        <v>30</v>
+        <v>0.1</v>
       </c>
       <c r="J2">
-        <v>5.1724138000000003E-2</v>
+        <v>30</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>5.1724138000000003E-2</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -549,32 +558,35 @@
       <c r="E3" s="1">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="F3">
-        <v>-0.5</v>
+      <c r="F3" s="1">
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="H3">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="I3">
-        <v>30</v>
+        <v>0.1</v>
       </c>
       <c r="J3">
-        <v>5.1724138000000003E-2</v>
+        <v>30</v>
       </c>
       <c r="K3">
-        <v>1</v>
+        <v>5.1724138000000003E-2</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -590,32 +602,35 @@
       <c r="E4" s="1">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="F4">
-        <v>-0.5</v>
+      <c r="F4" s="1">
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="H4">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="I4">
-        <v>30</v>
+        <v>0.1</v>
       </c>
       <c r="J4">
-        <v>5.1724138000000003E-2</v>
+        <v>30</v>
       </c>
       <c r="K4">
-        <v>1</v>
+        <v>5.1724138000000003E-2</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -631,32 +646,35 @@
       <c r="E5" s="1">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="F5">
-        <v>-0.5</v>
+      <c r="F5" s="1">
+        <v>1</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="H5">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="I5">
-        <v>30</v>
+        <v>0.1</v>
       </c>
       <c r="J5">
-        <v>5.1724138000000003E-2</v>
+        <v>30</v>
       </c>
       <c r="K5">
-        <v>1</v>
+        <v>5.1724138000000003E-2</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -672,32 +690,35 @@
       <c r="E6" s="1">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="F6">
-        <v>-0.5</v>
+      <c r="F6" s="1">
+        <v>1</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="H6">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="I6">
-        <v>30</v>
+        <v>0.1</v>
       </c>
       <c r="J6">
-        <v>5.1724138000000003E-2</v>
+        <v>30</v>
       </c>
       <c r="K6">
-        <v>1</v>
+        <v>5.1724138000000003E-2</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -713,32 +734,35 @@
       <c r="E7" s="1">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="F7">
-        <v>-0.5</v>
+      <c r="F7" s="1">
+        <v>1</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="H7">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="I7">
-        <v>30</v>
+        <v>0.1</v>
       </c>
       <c r="J7">
-        <v>5.1724138000000003E-2</v>
+        <v>30</v>
       </c>
       <c r="K7">
-        <v>1</v>
+        <v>5.1724138000000003E-2</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -754,32 +778,35 @@
       <c r="E8" s="1">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="F8">
-        <v>-0.5</v>
+      <c r="F8" s="1">
+        <v>1</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="H8">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="I8">
-        <v>30</v>
+        <v>0.1</v>
       </c>
       <c r="J8">
-        <v>5.1724138000000003E-2</v>
+        <v>30</v>
       </c>
       <c r="K8">
-        <v>1</v>
+        <v>5.1724138000000003E-2</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -795,32 +822,35 @@
       <c r="E9" s="1">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="F9">
-        <v>-0.5</v>
+      <c r="F9" s="1">
+        <v>1</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="H9">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="I9">
-        <v>30</v>
+        <v>0.1</v>
       </c>
       <c r="J9">
-        <v>5.1724138000000003E-2</v>
+        <v>30</v>
       </c>
       <c r="K9">
-        <v>1</v>
+        <v>5.1724138000000003E-2</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -836,32 +866,35 @@
       <c r="E10" s="1">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="F10">
-        <v>-0.5</v>
+      <c r="F10" s="1">
+        <v>1</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="H10">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="I10">
-        <v>30</v>
+        <v>0.1</v>
       </c>
       <c r="J10">
-        <v>5.1724138000000003E-2</v>
+        <v>30</v>
       </c>
       <c r="K10">
-        <v>1</v>
+        <v>5.1724138000000003E-2</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -877,32 +910,35 @@
       <c r="E11" s="1">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="F11">
-        <v>-0.5</v>
+      <c r="F11" s="1">
+        <v>1</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="H11">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="I11">
-        <v>30</v>
+        <v>0.1</v>
       </c>
       <c r="J11">
-        <v>5.1724138000000003E-2</v>
+        <v>30</v>
       </c>
       <c r="K11">
-        <v>1</v>
+        <v>5.1724138000000003E-2</v>
       </c>
       <c r="L11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -918,32 +954,35 @@
       <c r="E12" s="1">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="F12">
-        <v>-0.5</v>
+      <c r="F12" s="1">
+        <v>1</v>
       </c>
       <c r="G12">
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="H12">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="I12">
-        <v>30</v>
+        <v>0.1</v>
       </c>
       <c r="J12">
-        <v>5.1724138000000003E-2</v>
+        <v>30</v>
       </c>
       <c r="K12">
-        <v>1</v>
+        <v>5.1724138000000003E-2</v>
       </c>
       <c r="L12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -959,32 +998,35 @@
       <c r="E13" s="1">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="F13">
-        <v>-0.5</v>
+      <c r="F13" s="1">
+        <v>1</v>
       </c>
       <c r="G13">
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="H13">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="I13">
-        <v>30</v>
+        <v>0.1</v>
       </c>
       <c r="J13">
-        <v>5.1724138000000003E-2</v>
+        <v>30</v>
       </c>
       <c r="K13">
-        <v>1</v>
+        <v>5.1724138000000003E-2</v>
       </c>
       <c r="L13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1000,32 +1042,35 @@
       <c r="E14" s="1">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="F14">
-        <v>-0.5</v>
+      <c r="F14" s="1">
+        <v>1</v>
       </c>
       <c r="G14">
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="H14">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="I14">
-        <v>30</v>
+        <v>0.1</v>
       </c>
       <c r="J14">
-        <v>5.1724138000000003E-2</v>
+        <v>30</v>
       </c>
       <c r="K14">
-        <v>1</v>
+        <v>5.1724138000000003E-2</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1041,32 +1086,35 @@
       <c r="E15" s="1">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="F15">
-        <v>-0.5</v>
+      <c r="F15" s="1">
+        <v>1</v>
       </c>
       <c r="G15">
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="H15">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="I15">
-        <v>30</v>
+        <v>0.1</v>
       </c>
       <c r="J15">
-        <v>5.1724138000000003E-2</v>
+        <v>30</v>
       </c>
       <c r="K15">
-        <v>1</v>
+        <v>5.1724138000000003E-2</v>
       </c>
       <c r="L15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1082,28 +1130,31 @@
       <c r="E16" s="1">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="F16">
-        <v>-0.5</v>
+      <c r="F16" s="1">
+        <v>1</v>
       </c>
       <c r="G16">
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="H16">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="I16">
-        <v>30</v>
+        <v>0.1</v>
       </c>
       <c r="J16">
-        <v>5.1724138000000003E-2</v>
+        <v>30</v>
       </c>
       <c r="K16">
-        <v>1</v>
+        <v>5.1724138000000003E-2</v>
       </c>
       <c r="L16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
         <v>0</v>
       </c>
     </row>

</xml_diff>